<commit_message>
Lesson 17 Average Formula
</commit_message>
<xml_diff>
--- a/tutorial_03.xlsx
+++ b/tutorial_03.xlsx
@@ -9,17 +9,20 @@
   <sheets>
     <sheet name="Names and Colours" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Team</t>
   </si>
   <si>
     <t>Colour</t>
+  </si>
+  <si>
+    <t>League Position 2023</t>
   </si>
   <si>
     <t>Westham</t>
@@ -404,77 +407,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="C9">
+        <f>AVERAGE(C2:C8)</f>
+        <v>9.7142857142857135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lesson 17 Save function improved
</commit_message>
<xml_diff>
--- a/tutorial_03.xlsx
+++ b/tutorial_03.xlsx
@@ -503,8 +503,8 @@
     </row>
     <row r="9" spans="1:3">
       <c r="C9">
-        <f>AVERAGE(C2:C8)</f>
-        <v>9.7142857142857135</v>
+        <f>SUM(C2:C8)</f>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lesson 18 Cell formatting
</commit_message>
<xml_diff>
--- a/tutorial_03.xlsx
+++ b/tutorial_03.xlsx
@@ -71,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +82,12 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFAA0011"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -105,8 +111,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -412,15 +419,18 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="26.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -503,8 +513,8 @@
     </row>
     <row r="9" spans="1:3">
       <c r="C9">
-        <f>SUM(C2:C8)</f>
-        <v>68</v>
+        <f>AVERAGE(C2:C8)</f>
+        <v>9.7142857142857135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lesson 19 Cell format border
</commit_message>
<xml_diff>
--- a/tutorial_03.xlsx
+++ b/tutorial_03.xlsx
@@ -99,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -107,14 +107,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,12 +432,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25">
       <c r="A1" s="1" t="s">
@@ -512,7 +527,7 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="C9">
+      <c r="C9" s="3">
         <f>AVERAGE(C2:C8)</f>
         <v>9.7142857142857135</v>
       </c>

</xml_diff>

<commit_message>
Lesson 20 - Create a Pie Chart
</commit_message>
<xml_diff>
--- a/tutorial_03.xlsx
+++ b/tutorial_03.xlsx
@@ -1,105 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="540" windowWidth="11175" windowHeight="9150"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Names and Colours" sheetId="1" r:id="rId1"/>
+    <sheet name="Names and Colours" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Team</t>
-  </si>
-  <si>
-    <t>Colour</t>
-  </si>
-  <si>
-    <t>League Position 2023</t>
-  </si>
-  <si>
-    <t>Westham</t>
-  </si>
-  <si>
-    <t>Claret</t>
-  </si>
-  <si>
-    <t>Arsenal</t>
-  </si>
-  <si>
-    <t>Yellow</t>
-  </si>
-  <si>
-    <t>Chelsea</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Man Utd</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Newcastle</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Wolves</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>Leeds</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color rgb="FFAA0011"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -107,41 +45,86 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -429,107 +412,145 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Colour</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>League Position 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Westham</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Claret</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Man Utd</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Wolves</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8">
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Leeds</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="C9" s="3">
+    <row r="9">
+      <c r="C9">
         <f>AVERAGE(C2:C8)</f>
-        <v>9.7142857142857135</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>